<commit_message>
Top 20 nodes and edges
</commit_message>
<xml_diff>
--- a/Tulip_files/Simmelian_statistics.xlsx
+++ b/Tulip_files/Simmelian_statistics.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Simmelian_statistics_opencare.c" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Kcore" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Weighted Kcore" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Modularity Simmelian" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="top20" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="147">
   <si>
     <t xml:space="preserve">opencare</t>
   </si>
@@ -75,6 +76,396 @@
   <si>
     <t xml:space="preserve">weigth</t>
   </si>
+  <si>
+    <t xml:space="preserve">Opencare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">betweenness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">research question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lakedistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">community-based care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cumbria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doncaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yorkshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photooftheday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">participatory design/collaboration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">england</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existing system failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mental health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resource strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sustainability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">story sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenSource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self-care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instagood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">london</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autumn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">somerset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">summer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outside existing systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">youth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beautiful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skill sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vscocam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picoftheday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">care networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bawtry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meaningful life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">place-based</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intergenerational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landscape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edge_force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">research question - community-based care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conflict - resource strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cumbria - lakedistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yorkshire - beer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration - research question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grassroots - making rules for spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thegentlemansretreat - bawtry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue - glitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration - building relationships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medical research - nutrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bawtry - barbershop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">london - bluray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">community-based care - legality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legality - informal discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thegentlemansretreat - barbershop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">louth - nature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration - resource strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design intervention - falling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bawtry - themanclub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beer - view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resource strain - research question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wearable technology - design intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thegentlemansretreat - themanclub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yorkshire - fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resource strain - community-based care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration - politics of healthcare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">themanclub - barbershop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beer - northyorkshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legality - migration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration - design intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bawtry - apothecary87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trainerlife - picoftheday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existing system failure - legality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">governance - legality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thegentlemansretreat - apothecary87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bawtry - beer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migration - story sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design intervention - research question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">themanclub - apothecary87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fitness - lakedistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legality - research question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">holistic healthcare - conceptual framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thegentlemansretreat - barberlife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">love - saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">safety - regulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instagram - medical professionals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barbershop - apothecary87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yorkshirevapers - northyorkshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mental health - creativity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trauma - law enforcement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bawtry - barberlife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cumbria - fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mental health - art and (health)care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psychology of medical technology - trauma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barberlife - themanclub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photooftheday - london</t>
+  </si>
+  <si>
+    <t xml:space="preserve">research question - story sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cultural difference - map-making</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barberlife - barbershop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">london - yorkshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">methodology - community-based care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homemade paint - hands-on/DIY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barberlife - apothecary87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">london - homecinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legality - safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moringa - blood regulatory function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bawtry - tgr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">projector - london</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crisis - resource strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tinkering is easier when the device is cheaper - hands-on/DIY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thegentlemansretreat - tgr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fitness - somerset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation - legality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supporting not fixing - making rules for spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">themanclub - tgr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beer - camping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mental health - suicide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tolerance - social design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tgr - barbershop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">humberston - cleethorpes</t>
+  </si>
 </sst>
 </file>
 
@@ -84,7 +475,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -111,6 +502,11 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -182,11 +578,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1324,11 +1720,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53985146"/>
-        <c:axId val="42036221"/>
+        <c:axId val="65818154"/>
+        <c:axId val="53975494"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53985146"/>
+        <c:axId val="65818154"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1364,12 +1760,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42036221"/>
+        <c:crossAx val="53975494"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42036221"/>
+        <c:axId val="53975494"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1811,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53985146"/>
+        <c:crossAx val="65818154"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2514,11 +2910,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="74174196"/>
-        <c:axId val="67911897"/>
+        <c:axId val="72196586"/>
+        <c:axId val="71037473"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74174196"/>
+        <c:axId val="72196586"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2554,12 +2950,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67911897"/>
+        <c:crossAx val="71037473"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67911897"/>
+        <c:axId val="71037473"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2605,7 +3001,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74174196"/>
+        <c:crossAx val="72196586"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3761,11 +4157,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="67691521"/>
-        <c:axId val="23944221"/>
+        <c:axId val="79291297"/>
+        <c:axId val="31550680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67691521"/>
+        <c:axId val="79291297"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3801,12 +4197,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23944221"/>
+        <c:crossAx val="31550680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23944221"/>
+        <c:axId val="31550680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3852,7 +4248,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67691521"/>
+        <c:crossAx val="79291297"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5006,11 +5402,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="55677798"/>
-        <c:axId val="27329489"/>
+        <c:axId val="26835331"/>
+        <c:axId val="54204667"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55677798"/>
+        <c:axId val="26835331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5046,12 +5442,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27329489"/>
+        <c:crossAx val="54204667"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27329489"/>
+        <c:axId val="54204667"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5097,7 +5493,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55677798"/>
+        <c:crossAx val="26835331"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5296,11 +5692,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="58298140"/>
-        <c:axId val="26353405"/>
+        <c:axId val="42001288"/>
+        <c:axId val="77165416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58298140"/>
+        <c:axId val="42001288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5336,14 +5732,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26353405"/>
+        <c:crossAx val="77165416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26353405"/>
+        <c:axId val="77165416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5389,7 +5785,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58298140"/>
+        <c:crossAx val="42001288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5576,11 +5972,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="50569215"/>
-        <c:axId val="57951957"/>
+        <c:axId val="1449912"/>
+        <c:axId val="76848765"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50569215"/>
+        <c:axId val="1449912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5616,14 +6012,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57951957"/>
+        <c:crossAx val="76848765"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57951957"/>
+        <c:axId val="76848765"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5669,7 +6065,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50569215"/>
+        <c:crossAx val="1449912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5904,11 +6300,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55467236"/>
-        <c:axId val="86349920"/>
+        <c:axId val="82246118"/>
+        <c:axId val="85313982"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55467236"/>
+        <c:axId val="82246118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5944,14 +6340,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86349920"/>
+        <c:crossAx val="85313982"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86349920"/>
+        <c:axId val="85313982"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5997,7 +6393,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55467236"/>
+        <c:crossAx val="82246118"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6742,11 +7138,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="75589649"/>
-        <c:axId val="58436774"/>
+        <c:axId val="96515663"/>
+        <c:axId val="87966145"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75589649"/>
+        <c:axId val="96515663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6782,14 +7178,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58436774"/>
+        <c:crossAx val="87966145"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58436774"/>
+        <c:axId val="87966145"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6835,7 +7231,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75589649"/>
+        <c:crossAx val="96515663"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6883,9 +7279,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>634680</xdr:colOff>
+      <xdr:colOff>633960</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6893,8 +7289,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8978760" y="241200"/>
-        <a:ext cx="7581600" cy="5587560"/>
+        <a:off x="9550080" y="241200"/>
+        <a:ext cx="8095320" cy="5586840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6913,9 +7309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>647280</xdr:colOff>
+      <xdr:colOff>646560</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6923,8 +7319,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8991360" y="5918040"/>
-        <a:ext cx="7581600" cy="5625720"/>
+        <a:off x="9562680" y="5918040"/>
+        <a:ext cx="8095320" cy="5625000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6943,9 +7339,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>749160</xdr:colOff>
+      <xdr:colOff>748440</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6953,8 +7349,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17068680" y="4305240"/>
-        <a:ext cx="4635360" cy="2743200"/>
+        <a:off x="18211680" y="4305240"/>
+        <a:ext cx="4920480" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6973,9 +7369,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>25200</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6983,8 +7379,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17170200" y="9232920"/>
-        <a:ext cx="4647960" cy="2742840"/>
+        <a:off x="18313200" y="9232920"/>
+        <a:ext cx="4990320" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7008,9 +7404,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>571320</xdr:colOff>
+      <xdr:colOff>570600</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7018,8 +7414,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="965160" y="8102520"/>
-        <a:ext cx="4635360" cy="2743200"/>
+        <a:off x="1022400" y="8102520"/>
+        <a:ext cx="4920120" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7038,9 +7434,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>50400</xdr:colOff>
+      <xdr:colOff>49680</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7048,8 +7444,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7137000" y="8153280"/>
-        <a:ext cx="4647960" cy="2743200"/>
+        <a:off x="7594200" y="8153280"/>
+        <a:ext cx="4990320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7073,9 +7469,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>419400</xdr:colOff>
+      <xdr:colOff>418680</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7084,7 +7480,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="800280" y="8699400"/>
-        <a:ext cx="5194800" cy="2742840"/>
+        <a:ext cx="5552280" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7103,9 +7499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>812520</xdr:colOff>
+      <xdr:colOff>811800</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>100800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7113,8 +7509,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12513240" y="7086600"/>
-        <a:ext cx="4790160" cy="2742840"/>
+        <a:off x="13274640" y="7086600"/>
+        <a:ext cx="5063040" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7140,7 +7536,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9320,7 +9716,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10801,15 +11197,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.893023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8325581395349"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.893023255814"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8325581395349"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16623,23 +17019,23 @@
   </sheetPr>
   <dimension ref="B1:N12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.5023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1116279069767"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.5023255813953"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.6046511627907"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3674418604651"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.1116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8744186046512"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.8744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16995,4 +17391,1114 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M45"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.753488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4651162790698"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.5767441860465"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.893023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.706976744186"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>353</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>47230.1769163</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>307</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>194109.218623</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>45931.2935821</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>302</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>169907.925459</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>252</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>33484.0121866</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>296</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>169234.078934</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>28559.9297199</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>276</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>167930.819144</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>207</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>20259.3309153</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>152372.254934</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>18396.7449126</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>116517.73459</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>18201.6317347</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>248</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>116455.52327</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>17970.4238949</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>233</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>115651.48626</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>17185.3229219</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>111755.090618</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>16045.663783</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>106343.338891</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>15514.6669225</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>101469.14643</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>15269.9348831</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>90807.2312481</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>13828.0824899</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>81590.2690378</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>12485.1297653</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>73216.1552298</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>9116.73355706</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>72370.9795224</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>9102.77860101</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>69732.6299631</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>8877.96368386</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>65086.7064403</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>8467.05745516</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>63939.8904461</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>8098.45290202</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>60498.0279691</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>7688.34130805</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>60462.5935553</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2044.99936283</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>277</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>43411.9606449</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1976</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>38398.1598062</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1976</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>24442.0897601</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1976</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>23930.2236418</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>1377.65351504</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>22979.44499</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>1129.40809968</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>22811.1542731</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>1119.5141744</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>18415.3547227</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>1074.50991458</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>18272.8558043</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1051.18912577</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>17954.6204214</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1009.49255368</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <v>16643.1789459</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <v>16413.4765776</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>16296</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <v>15339.1705661</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <v>15288.4480468</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>15167.2503872</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>14945.9185136</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>14945.9185136</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>14896.6659868</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <v>14511.9284747</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>989</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>14266</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>